<commit_message>
Excel Updater, Sudoku, + various updates.
</commit_message>
<xml_diff>
--- a/xl/transactions.xlsx
+++ b/xl/transactions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7K\Documents\Python\master-python101\xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F5F747-32C8-4E90-8DD1-1B631CC7EB3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A26602C-6844-4730-9FC7-20352360A5CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -371,18 +371,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="11.5546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -392,9 +390,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1"/>
     </row>
-    <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1001</v>
       </c>
@@ -404,9 +401,8 @@
       <c r="C2" s="2">
         <v>5.95</v>
       </c>
-      <c r="D2"/>
     </row>
-    <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1002</v>
       </c>
@@ -416,9 +412,8 @@
       <c r="C3" s="2">
         <v>6.95</v>
       </c>
-      <c r="D3"/>
     </row>
-    <row r="4" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1003</v>
       </c>
@@ -428,7 +423,6 @@
       <c r="C4" s="2">
         <v>7.95</v>
       </c>
-      <c r="D4"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>